<commit_message>
Update files for website
</commit_message>
<xml_diff>
--- a/planning244_s25.xlsx
+++ b/planning244_s25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinbelton/Repositories/M244-Spring25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A29278-041D-0447-B38C-72432EE49D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772282EC-530E-5845-ACA7-2ED05BC75807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="123">
   <si>
     <t>Date</t>
   </si>
@@ -77,19 +77,12 @@
     <t>R vs Python</t>
   </si>
   <si>
-    <t xml:space="preserve">- Download and install R and Rstudio. See instructions in Section 1.1.1  &lt;a href="https://moderndive.netlify.app/1-getting-started.html#installing"&gt;here&lt;/a&gt; 
-&lt;br&gt; - Download and install the Anaconda Distribution (for Python). See instructions &lt;a href="https://docs.anaconda.com/anaconda/install/index.html"&gt;here&lt;/a&gt;  </t>
-  </si>
-  <si>
     <t>Data Science in Python and R</t>
   </si>
   <si>
     <t xml:space="preserve"> - &lt;a href="https://rstudio.github.io/reticulate/articles/python_primer.html"&gt; Primer on Python for R Users &lt;/a&gt;    </t>
   </si>
   <si>
-    <t>- Yale GPA vs Majors Response Essay</t>
-  </si>
-  <si>
     <t>Manipulating Data in R and Python</t>
   </si>
   <si>
@@ -310,9 +303,6 @@
   </si>
   <si>
     <t xml:space="preserve"> - Syllabus </t>
-  </si>
-  <si>
-    <t>- Course Info Sheet</t>
   </si>
   <si>
     <t>Visualization in R and Python</t>
@@ -413,6 +403,9 @@
   <si>
     <t xml:space="preserve"> - &lt;a href="https://r4ds.hadley.nz/workflow-basics"&gt;R4DS Ch. 2&lt;/a&gt;  &lt;br&gt; - ISLP 2.3 &lt;br&gt; - &lt;a href="https://www.datacamp.com/blog/python-vs-r-for-data-science-whats-the-difference"&gt;Python vs R for Data Science&lt;/a&gt; 
 &lt;br&gt; - Review R vs Python Slides (on Moodle)</t>
+  </si>
+  <si>
+    <t>- Course Info Sheet &lt;br&gt; - Download and install R, Rstudio, and Python</t>
   </si>
 </sst>
 </file>
@@ -696,7 +689,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -713,7 +706,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -751,10 +744,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -775,7 +768,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>10</v>
@@ -796,12 +789,10 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -818,14 +809,12 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -842,7 +831,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -859,14 +848,14 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
@@ -903,16 +892,16 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -928,13 +917,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F10" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -951,13 +940,13 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -974,10 +963,10 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -995,16 +984,16 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1017,20 +1006,20 @@
         <v>45722</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4">
         <f>B14+5</f>
@@ -1038,17 +1027,17 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B16" s="4">
         <f>B15+2</f>
@@ -1056,17 +1045,17 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B17" s="4">
         <f>B16+5</f>
@@ -1074,17 +1063,17 @@
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B18" s="4">
         <f>B17+2</f>
@@ -1092,10 +1081,10 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1113,13 +1102,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1132,19 +1121,19 @@
         <v>45743</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1160,13 +1149,13 @@
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1180,19 +1169,19 @@
         <v>45750</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1208,16 +1197,16 @@
         <v>6</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1230,16 +1219,16 @@
         <v>45757</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1255,16 +1244,16 @@
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1277,16 +1266,16 @@
         <v>45764</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F26" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1299,17 +1288,17 @@
         <v>45769</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1322,13 +1311,13 @@
         <v>45771</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -1342,19 +1331,19 @@
         <v>45776</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1367,13 +1356,13 @@
         <v>45778</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1388,13 +1377,13 @@
         <v>45783</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="3"/>
@@ -2503,197 +2492,197 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H15" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G16" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="7:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G17" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="7:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="7:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>